<commit_message>
Final Commit before delivery
</commit_message>
<xml_diff>
--- a/person_details.xlsx
+++ b/person_details.xlsx
@@ -30,7 +30,7 @@
     <t>Indian</t>
   </si>
   <si>
-    <t>Female</t>
+    <t>Priya</t>
   </si>
 </sst>
 </file>
@@ -94,7 +94,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -141,7 +141,7 @@
     <row r="2" spans="1:6" ht="13.5">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Burhan</t>
+          <t>Akash</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -165,13 +165,13 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Nidhi</t>
-        </is>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
       </c>
       <c r="C3" t="s">
         <v>0</v>

</xml_diff>